<commit_message>
Working on the Loop
</commit_message>
<xml_diff>
--- a/Projektarbeit/Dokumentation/Stundenliste.xlsx
+++ b/Projektarbeit/Dokumentation/Stundenliste.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20378"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20379"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0ABC6A96-0B59-4D6E-8A73-F518FE76827B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC8BDCEF-88BA-436B-A8C6-3039F1A3A009}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14025" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -388,7 +388,7 @@
   <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -440,7 +440,12 @@
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B8" s="1"/>
+      <c r="B8" s="2">
+        <v>44505</v>
+      </c>
+      <c r="C8">
+        <v>2</v>
+      </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B9" s="1"/>

</xml_diff>

<commit_message>
Test Data Matlab NN
</commit_message>
<xml_diff>
--- a/Projektarbeit/Dokumentation/Stundenliste.xlsx
+++ b/Projektarbeit/Dokumentation/Stundenliste.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20380"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CED033E-C44C-446D-B38D-378E989B2A46}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DD9C7EC-9BD4-46EF-ABF2-F1C49D02A994}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14025" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -388,7 +388,7 @@
   <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -472,13 +472,25 @@
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B12" s="1"/>
+      <c r="B12" s="2">
+        <v>44524</v>
+      </c>
+      <c r="C12">
+        <v>2</v>
+      </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B13" s="1"/>
+      <c r="B13" s="2">
+        <v>44525</v>
+      </c>
+      <c r="C13">
+        <v>3</v>
+      </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B14" s="1"/>
+      <c r="B14" s="2">
+        <v>44527</v>
+      </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B15" s="1"/>

</xml_diff>